<commit_message>
Task 14: add group/contacts random data generator
</commit_message>
<xml_diff>
--- a/addressbook-web-tests/addressbook-web-tests/groups.xlsx
+++ b/addressbook-web-tests/addressbook-web-tests/groups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Source\Repos\csharp_training\addressbook-web-tests\addressbook-test-data-generators\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Source\Repos\csharp_training\addressbook-web-tests\addressbook-web-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,33 +359,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>